<commit_message>
[add]: <oop + avtomaty + interfaces>
</commit_message>
<xml_diff>
--- a/semester_4/TeoriyaAvtomatov/lab0/l0.xlsx
+++ b/semester_4/TeoriyaAvtomatov/lab0/l0.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE9BEB4F-EF82-45BF-B336-2ADA65961E10}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6DBADF-889A-4381-A254-4123F0F0BCBC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
   <si>
     <t>10cc</t>
   </si>
@@ -175,9 +175,6 @@
   </si>
   <si>
     <t>-x3</t>
-  </si>
-  <si>
-    <t>(x3*x5) + (x4*-x2*-x5) + (x1*-x3*-x5) + (-x3*-x4*x5) * (x3*-x2)</t>
   </si>
 </sst>
 </file>
@@ -431,7 +428,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -458,7 +455,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -576,36 +572,36 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -615,22 +611,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -652,60 +648,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>31</xdr:col>
-          <xdr:colOff>400050</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>34</xdr:col>
-          <xdr:colOff>390525</xdr:colOff>
-          <xdr:row>9</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1025" name="Object 1" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1025"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
@@ -724,7 +666,7 @@
         <xdr:cNvPr id="2" name="Рисунок 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEBD7939-7E9F-4DD0-8D97-AB335C2B6906}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -768,7 +710,7 @@
         <xdr:cNvPr id="3" name="Рисунок 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47E82EB0-E77E-449A-A8C3-832B4606D2BA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1059,11 +1001,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AK47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,42 +1014,42 @@
     <col min="21" max="30" width="4.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+    <row r="1" spans="1:37" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="71" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="Q1" s="27"/>
-    </row>
-    <row r="2" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="V2" s="28" t="s">
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="Q1" s="26"/>
+    </row>
+    <row r="2" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V2" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="W2" s="28" t="s">
+      <c r="W2" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="X2" s="28" t="s">
+      <c r="X2" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="Y2" s="28" t="s">
+      <c r="Y2" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="Z2" s="28" t="s">
+      <c r="Z2" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="AA2" s="28" t="s">
+      <c r="AA2" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="AB2" s="28" t="s">
+      <c r="AB2" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="AC2" s="28" t="s">
+      <c r="AC2" s="27" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1115,27 +1057,27 @@
         <v>1</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="U3" s="28" t="s">
+      <c r="U3" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="V3" s="36">
-        <v>1</v>
-      </c>
-      <c r="W3" s="37"/>
-      <c r="X3" s="37"/>
-      <c r="Y3" s="37"/>
-      <c r="Z3" s="37"/>
-      <c r="AA3" s="37">
-        <v>1</v>
-      </c>
-      <c r="AB3" s="37">
-        <v>1</v>
-      </c>
-      <c r="AC3" s="38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="V3" s="35">
+        <v>1</v>
+      </c>
+      <c r="W3" s="36"/>
+      <c r="X3" s="36"/>
+      <c r="Y3" s="36"/>
+      <c r="Z3" s="36"/>
+      <c r="AA3" s="36">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="36">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1145,29 +1087,29 @@
       <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="U4" s="28" t="s">
+      <c r="U4" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="V4" s="30">
-        <v>1</v>
-      </c>
-      <c r="W4" s="31"/>
-      <c r="X4" s="31"/>
-      <c r="Y4" s="31">
-        <v>1</v>
-      </c>
-      <c r="Z4" s="31"/>
-      <c r="AA4" s="31">
-        <v>1</v>
-      </c>
-      <c r="AB4" s="31">
-        <v>1</v>
-      </c>
-      <c r="AC4" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="V4" s="29">
+        <v>1</v>
+      </c>
+      <c r="W4" s="30"/>
+      <c r="X4" s="30"/>
+      <c r="Y4" s="30">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="30"/>
+      <c r="AA4" s="30">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="30">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>5</v>
       </c>
@@ -1177,23 +1119,23 @@
       <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="U5" s="28" t="s">
+      <c r="U5" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="V5" s="30">
-        <v>1</v>
-      </c>
-      <c r="W5" s="31"/>
-      <c r="X5" s="31"/>
-      <c r="Y5" s="31">
-        <v>1</v>
-      </c>
-      <c r="Z5" s="31"/>
-      <c r="AA5" s="31"/>
-      <c r="AB5" s="31"/>
-      <c r="AC5" s="32"/>
-    </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="V5" s="29">
+        <v>1</v>
+      </c>
+      <c r="W5" s="30"/>
+      <c r="X5" s="30"/>
+      <c r="Y5" s="30">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="30"/>
+      <c r="AA5" s="30"/>
+      <c r="AB5" s="30"/>
+      <c r="AC5" s="31"/>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>8</v>
       </c>
@@ -1203,23 +1145,23 @@
       <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="U6" s="28" t="s">
+      <c r="U6" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="V6" s="33">
-        <v>1</v>
-      </c>
-      <c r="W6" s="34"/>
-      <c r="X6" s="34"/>
-      <c r="Y6" s="34"/>
-      <c r="Z6" s="34"/>
-      <c r="AA6" s="34"/>
-      <c r="AB6" s="34"/>
-      <c r="AC6" s="35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="V6" s="32">
+        <v>1</v>
+      </c>
+      <c r="W6" s="33"/>
+      <c r="X6" s="33"/>
+      <c r="Y6" s="33"/>
+      <c r="Z6" s="33"/>
+      <c r="AA6" s="33"/>
+      <c r="AB6" s="33"/>
+      <c r="AC6" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>10</v>
       </c>
@@ -1229,28 +1171,28 @@
       <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="Y7" s="29"/>
-    </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="Y7" s="28"/>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>11</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="U8" s="64" t="s">
+      <c r="U8" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="V8" s="74"/>
-      <c r="W8" s="74"/>
-      <c r="X8" s="74"/>
-      <c r="Y8" s="74"/>
-      <c r="Z8" s="74"/>
-      <c r="AA8" s="74"/>
-      <c r="AB8" s="74"/>
-      <c r="AC8" s="74"/>
-    </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="V8" s="73"/>
+      <c r="W8" s="73"/>
+      <c r="X8" s="73"/>
+      <c r="Y8" s="73"/>
+      <c r="Z8" s="73"/>
+      <c r="AA8" s="73"/>
+      <c r="AB8" s="73"/>
+      <c r="AC8" s="73"/>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>12</v>
       </c>
@@ -1258,152 +1200,167 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>14</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="V10" s="71" t="s">
+      <c r="V10" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="W10" s="72"/>
-      <c r="X10" s="72"/>
-      <c r="Y10" s="72"/>
-      <c r="Z10" s="71" t="s">
+      <c r="W10" s="70"/>
+      <c r="X10" s="70"/>
+      <c r="Y10" s="70"/>
+      <c r="Z10" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="AA10" s="72"/>
-      <c r="AB10" s="72"/>
-      <c r="AC10" s="72"/>
-    </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="U11" s="39"/>
-      <c r="V11" s="75" t="s">
+      <c r="AA10" s="70"/>
+      <c r="AB10" s="70"/>
+      <c r="AC10" s="70"/>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="U11" s="38"/>
+      <c r="V11" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="W11" s="76"/>
-      <c r="X11" s="75" t="s">
+      <c r="W11" s="75"/>
+      <c r="X11" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="Y11" s="76"/>
-      <c r="Z11" s="75" t="s">
+      <c r="Y11" s="75"/>
+      <c r="Z11" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="AA11" s="76"/>
-      <c r="AB11" s="75" t="s">
+      <c r="AA11" s="75"/>
+      <c r="AB11" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="AC11" s="76"/>
-      <c r="AD11" s="39"/>
-      <c r="AE11" s="64" t="s">
-        <v>44</v>
-      </c>
-      <c r="AF11" s="64"/>
-      <c r="AG11" s="64"/>
-      <c r="AH11" s="64"/>
-      <c r="AI11" s="64"/>
-      <c r="AJ11" s="64"/>
-    </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="B12" s="26" t="s">
+      <c r="AC11" s="75"/>
+      <c r="AD11" s="38"/>
+      <c r="AE11" s="72"/>
+      <c r="AF11" s="72"/>
+      <c r="AG11" s="72"/>
+      <c r="AH11" s="72"/>
+      <c r="AI11" s="72"/>
+      <c r="AJ11" s="72"/>
+      <c r="AK11" s="72"/>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B12" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="19"/>
-      <c r="O12" s="21"/>
-      <c r="P12" s="20"/>
-      <c r="Q12" s="20"/>
-      <c r="R12" s="20"/>
-      <c r="S12" s="20"/>
-      <c r="U12" s="69" t="s">
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
+      <c r="U12" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="V12" s="40"/>
-      <c r="W12" s="49">
-        <v>0</v>
-      </c>
-      <c r="X12" s="50">
-        <v>0</v>
-      </c>
-      <c r="Y12" s="52">
-        <v>0</v>
-      </c>
-      <c r="Z12" s="53">
-        <v>0</v>
-      </c>
-      <c r="AA12" s="41"/>
-      <c r="AB12" s="41"/>
-      <c r="AC12" s="42"/>
-      <c r="AD12" s="17" t="s">
+      <c r="V12" s="39"/>
+      <c r="W12" s="48">
+        <v>0</v>
+      </c>
+      <c r="X12" s="49">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="51">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="52">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="40"/>
+      <c r="AB12" s="40"/>
+      <c r="AC12" s="41"/>
+      <c r="AD12" s="16" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A13" s="22"/>
+      <c r="AE12" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF12" s="73"/>
+      <c r="AG12" s="73"/>
+      <c r="AH12" s="73"/>
+      <c r="AI12" s="73"/>
+      <c r="AJ12" s="73"/>
+      <c r="AK12" s="73"/>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A13" s="21"/>
       <c r="C13" s="4"/>
-      <c r="D13" s="79" t="s">
+      <c r="D13" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="80"/>
-      <c r="F13" s="79" t="s">
+      <c r="E13" s="64"/>
+      <c r="F13" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="80"/>
+      <c r="G13" s="64"/>
       <c r="H13" s="4"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="81" t="s">
+      <c r="I13" s="19"/>
+      <c r="J13" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="K13" s="81"/>
-      <c r="L13" s="81"/>
-      <c r="M13" s="81"/>
-      <c r="N13" s="82"/>
-      <c r="O13" s="21"/>
-      <c r="P13" s="20"/>
-      <c r="Q13" s="20"/>
-      <c r="R13" s="20"/>
-      <c r="S13" s="20"/>
-      <c r="U13" s="70"/>
-      <c r="V13" s="43"/>
-      <c r="W13" s="51">
-        <v>0</v>
-      </c>
-      <c r="X13" s="48">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="44"/>
-      <c r="Z13" s="54">
-        <v>0</v>
-      </c>
-      <c r="AA13" s="44"/>
-      <c r="AB13" s="44"/>
-      <c r="AC13" s="45"/>
-      <c r="AD13" s="65" t="s">
+      <c r="K13" s="67"/>
+      <c r="L13" s="67"/>
+      <c r="M13" s="67"/>
+      <c r="N13" s="68"/>
+      <c r="O13" s="20"/>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="19"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="19"/>
+      <c r="U13" s="79"/>
+      <c r="V13" s="42"/>
+      <c r="W13" s="50">
+        <v>0</v>
+      </c>
+      <c r="X13" s="47">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="43"/>
+      <c r="Z13" s="53">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="43"/>
+      <c r="AB13" s="43"/>
+      <c r="AC13" s="44"/>
+      <c r="AD13" s="76" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="77" t="s">
+      <c r="AE13" s="72"/>
+      <c r="AF13" s="73"/>
+      <c r="AG13" s="73"/>
+      <c r="AH13" s="73"/>
+      <c r="AI13" s="73"/>
+      <c r="AJ13" s="73"/>
+      <c r="AK13" s="73"/>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A14" s="20"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="16">
-        <v>1</v>
-      </c>
-      <c r="E14" s="15">
+      <c r="D14" s="15">
+        <v>1</v>
+      </c>
+      <c r="E14" s="14">
         <v>1</v>
       </c>
       <c r="F14" s="4"/>
@@ -1411,150 +1368,150 @@
       <c r="H14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I14" s="20"/>
-      <c r="J14" s="81" t="s">
+      <c r="I14" s="19"/>
+      <c r="J14" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="K14" s="81"/>
-      <c r="L14" s="81"/>
-      <c r="M14" s="81"/>
-      <c r="N14" s="82"/>
-      <c r="O14" s="21"/>
-      <c r="P14" s="20"/>
-      <c r="Q14" s="20"/>
-      <c r="R14" s="20"/>
-      <c r="S14" s="20"/>
-      <c r="U14" s="69" t="s">
+      <c r="K14" s="67"/>
+      <c r="L14" s="67"/>
+      <c r="M14" s="67"/>
+      <c r="N14" s="68"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="19"/>
+      <c r="U14" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="V14" s="43"/>
-      <c r="W14" s="62">
-        <v>0</v>
-      </c>
-      <c r="X14" s="63">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="44"/>
-      <c r="Z14" s="56">
-        <v>0</v>
-      </c>
-      <c r="AA14" s="58">
-        <v>0</v>
-      </c>
-      <c r="AB14" s="59">
-        <v>0</v>
-      </c>
-      <c r="AC14" s="57">
-        <v>0</v>
-      </c>
-      <c r="AD14" s="66"/>
-    </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="78"/>
+      <c r="V14" s="42"/>
+      <c r="W14" s="61">
+        <v>0</v>
+      </c>
+      <c r="X14" s="62">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="43"/>
+      <c r="Z14" s="55">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="57">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="58">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="56">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="77"/>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A15" s="20"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="66"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="11">
-        <v>1</v>
-      </c>
-      <c r="H15" s="77" t="s">
+      <c r="G15" s="10">
+        <v>1</v>
+      </c>
+      <c r="H15" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="I15" s="20"/>
-      <c r="J15" s="81" t="s">
+      <c r="I15" s="19"/>
+      <c r="J15" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="K15" s="81"/>
-      <c r="L15" s="81"/>
-      <c r="M15" s="81"/>
-      <c r="N15" s="82"/>
-      <c r="O15" s="21"/>
-      <c r="P15" s="20"/>
-      <c r="Q15" s="20"/>
-      <c r="R15" s="20"/>
-      <c r="S15" s="20"/>
-      <c r="U15" s="70"/>
-      <c r="V15" s="46"/>
-      <c r="W15" s="60">
-        <v>0</v>
-      </c>
-      <c r="X15" s="61">
-        <v>0</v>
-      </c>
-      <c r="Y15" s="52">
-        <v>0</v>
-      </c>
-      <c r="Z15" s="55">
-        <v>0</v>
-      </c>
-      <c r="AA15" s="60">
-        <v>0</v>
-      </c>
-      <c r="AB15" s="61">
-        <v>0</v>
-      </c>
-      <c r="AC15" s="47"/>
-      <c r="AD15" s="17" t="s">
+      <c r="K15" s="67"/>
+      <c r="L15" s="67"/>
+      <c r="M15" s="67"/>
+      <c r="N15" s="68"/>
+      <c r="O15" s="20"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="19"/>
+      <c r="U15" s="79"/>
+      <c r="V15" s="45"/>
+      <c r="W15" s="59">
+        <v>0</v>
+      </c>
+      <c r="X15" s="60">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="51">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="54">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="59">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="60">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="46"/>
+      <c r="AD15" s="16" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="77" t="s">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A16" s="20"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="65" t="s">
         <v>17</v>
       </c>
       <c r="D16" s="4"/>
-      <c r="E16" s="14">
+      <c r="E16" s="13">
         <v>1</v>
       </c>
       <c r="F16" s="4"/>
-      <c r="G16" s="13">
-        <v>1</v>
-      </c>
-      <c r="H16" s="78"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="20"/>
-      <c r="M16" s="20"/>
-      <c r="N16" s="22"/>
-      <c r="O16" s="21"/>
-      <c r="P16" s="20"/>
-      <c r="Q16" s="20"/>
-      <c r="R16" s="20"/>
-      <c r="S16" s="20"/>
-      <c r="V16" s="10" t="s">
+      <c r="G16" s="12">
+        <v>1</v>
+      </c>
+      <c r="H16" s="66"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="21"/>
+      <c r="O16" s="20"/>
+      <c r="P16" s="19"/>
+      <c r="Q16" s="19"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="19"/>
+      <c r="V16" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="W16" s="67" t="s">
+      <c r="W16" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="X16" s="68"/>
-      <c r="Y16" s="10" t="s">
+      <c r="X16" s="81"/>
+      <c r="Y16" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="Z16" s="10" t="s">
+      <c r="Z16" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="AA16" s="67" t="s">
+      <c r="AA16" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="AB16" s="68"/>
-      <c r="AC16" s="10" t="s">
+      <c r="AB16" s="81"/>
+      <c r="AC16" s="27" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="78"/>
-      <c r="D17" s="16">
-        <v>1</v>
-      </c>
-      <c r="E17" s="14">
+      <c r="A17" s="20"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="15">
+        <v>1</v>
+      </c>
+      <c r="E17" s="13">
         <v>1</v>
       </c>
       <c r="F17" s="4"/>
@@ -1562,282 +1519,282 @@
       <c r="H17" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
-      <c r="L17" s="20"/>
-      <c r="M17" s="20"/>
-      <c r="N17" s="22"/>
-      <c r="O17" s="21"/>
-      <c r="P17" s="20"/>
-      <c r="Q17" s="20"/>
-      <c r="R17" s="20"/>
-      <c r="S17" s="20"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="21"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="19"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="19"/>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
-      <c r="B18" s="21"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="20"/>
       <c r="C18" s="4"/>
       <c r="D18" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="79" t="s">
+      <c r="E18" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="80"/>
+      <c r="F18" s="64"/>
       <c r="G18" s="8" t="s">
         <v>14</v>
       </c>
       <c r="H18" s="4"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="20"/>
-      <c r="N18" s="22"/>
-      <c r="O18" s="21"/>
-      <c r="P18" s="20"/>
-      <c r="Q18" s="20"/>
-      <c r="R18" s="20"/>
-      <c r="S18" s="20"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="20"/>
+      <c r="P18" s="19"/>
+      <c r="Q18" s="19"/>
+      <c r="R18" s="19"/>
+      <c r="S18" s="19"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="24"/>
-      <c r="N19" s="25"/>
-      <c r="O19" s="21"/>
-      <c r="P19" s="20"/>
-      <c r="Q19" s="20"/>
-      <c r="R19" s="20"/>
-      <c r="S19" s="20"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="20"/>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="19"/>
+      <c r="R19" s="19"/>
+      <c r="S19" s="19"/>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
+      <c r="A20" s="19"/>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
-      <c r="B21" s="26" t="s">
+      <c r="A21" s="21"/>
+      <c r="B21" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
-      <c r="N21" s="18"/>
-      <c r="O21" s="21"/>
-      <c r="P21" s="20"/>
-      <c r="Q21" s="20"/>
-      <c r="R21" s="20"/>
-      <c r="S21" s="20"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
+      <c r="O21" s="20"/>
+      <c r="P21" s="19"/>
+      <c r="Q21" s="19"/>
+      <c r="R21" s="19"/>
+      <c r="S21" s="19"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="20"/>
+      <c r="A22" s="21"/>
+      <c r="B22" s="19"/>
       <c r="C22" s="4"/>
-      <c r="D22" s="79" t="s">
+      <c r="D22" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="80"/>
-      <c r="F22" s="79" t="s">
+      <c r="E22" s="64"/>
+      <c r="F22" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="G22" s="80"/>
+      <c r="G22" s="64"/>
       <c r="H22" s="4"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="81" t="s">
+      <c r="I22" s="19"/>
+      <c r="J22" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="K22" s="81"/>
-      <c r="L22" s="81"/>
-      <c r="M22" s="81"/>
-      <c r="N22" s="81"/>
-      <c r="O22" s="21"/>
-      <c r="P22" s="20"/>
-      <c r="Q22" s="20"/>
-      <c r="R22" s="20"/>
-      <c r="S22" s="20"/>
+      <c r="K22" s="67"/>
+      <c r="L22" s="67"/>
+      <c r="M22" s="67"/>
+      <c r="N22" s="67"/>
+      <c r="O22" s="20"/>
+      <c r="P22" s="19"/>
+      <c r="Q22" s="19"/>
+      <c r="R22" s="19"/>
+      <c r="S22" s="19"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="77" t="s">
+      <c r="A23" s="21"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="65" t="s">
         <v>16</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
-      <c r="F23" s="14">
-        <v>0</v>
-      </c>
-      <c r="G23" s="15">
+      <c r="F23" s="13">
+        <v>0</v>
+      </c>
+      <c r="G23" s="14">
         <v>0</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I23" s="20"/>
-      <c r="J23" s="81" t="s">
+      <c r="I23" s="19"/>
+      <c r="J23" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="K23" s="81"/>
-      <c r="L23" s="81"/>
-      <c r="M23" s="81"/>
-      <c r="N23" s="81"/>
-      <c r="O23" s="21"/>
-      <c r="P23" s="20"/>
-      <c r="Q23" s="20"/>
-      <c r="R23" s="20"/>
-      <c r="S23" s="20"/>
+      <c r="K23" s="67"/>
+      <c r="L23" s="67"/>
+      <c r="M23" s="67"/>
+      <c r="N23" s="67"/>
+      <c r="O23" s="20"/>
+      <c r="P23" s="19"/>
+      <c r="Q23" s="19"/>
+      <c r="R23" s="19"/>
+      <c r="S23" s="19"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="78"/>
-      <c r="D24" s="14">
-        <v>0</v>
-      </c>
-      <c r="E24" s="15">
-        <v>0</v>
-      </c>
-      <c r="F24" s="12">
+      <c r="A24" s="21"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="66"/>
+      <c r="D24" s="13">
+        <v>0</v>
+      </c>
+      <c r="E24" s="14">
+        <v>0</v>
+      </c>
+      <c r="F24" s="11">
         <v>0</v>
       </c>
       <c r="G24" s="9"/>
-      <c r="H24" s="77" t="s">
+      <c r="H24" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="I24" s="20"/>
-      <c r="J24" s="81" t="s">
+      <c r="I24" s="19"/>
+      <c r="J24" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="K24" s="81"/>
-      <c r="L24" s="81"/>
-      <c r="M24" s="81"/>
-      <c r="N24" s="81"/>
-      <c r="O24" s="21"/>
-      <c r="P24" s="20"/>
-      <c r="Q24" s="20"/>
-      <c r="R24" s="20"/>
-      <c r="S24" s="20"/>
+      <c r="K24" s="67"/>
+      <c r="L24" s="67"/>
+      <c r="M24" s="67"/>
+      <c r="N24" s="67"/>
+      <c r="O24" s="20"/>
+      <c r="P24" s="19"/>
+      <c r="Q24" s="19"/>
+      <c r="R24" s="19"/>
+      <c r="S24" s="19"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="77" t="s">
+      <c r="A25" s="21"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="D25" s="13">
+      <c r="D25" s="12">
         <v>0</v>
       </c>
       <c r="E25" s="9"/>
-      <c r="F25" s="12">
+      <c r="F25" s="11">
         <v>0</v>
       </c>
       <c r="G25" s="9"/>
-      <c r="H25" s="78"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="20"/>
-      <c r="M25" s="20"/>
-      <c r="N25" s="20"/>
-      <c r="O25" s="21"/>
-      <c r="P25" s="20"/>
-      <c r="Q25" s="20"/>
-      <c r="R25" s="20"/>
-      <c r="S25" s="20"/>
+      <c r="H25" s="66"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="20"/>
+      <c r="P25" s="19"/>
+      <c r="Q25" s="19"/>
+      <c r="R25" s="19"/>
+      <c r="S25" s="19"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="78"/>
+      <c r="A26" s="21"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="66"/>
       <c r="D26" s="9"/>
       <c r="E26" s="9"/>
-      <c r="F26" s="14">
-        <v>0</v>
-      </c>
-      <c r="G26" s="15">
+      <c r="F26" s="13">
+        <v>0</v>
+      </c>
+      <c r="G26" s="14">
         <v>0</v>
       </c>
       <c r="H26" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
-      <c r="L26" s="20"/>
-      <c r="M26" s="20"/>
-      <c r="N26" s="20"/>
-      <c r="O26" s="21"/>
-      <c r="P26" s="20"/>
-      <c r="Q26" s="20"/>
-      <c r="R26" s="20"/>
-      <c r="S26" s="20"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="20"/>
+      <c r="P26" s="19"/>
+      <c r="Q26" s="19"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="19"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
-      <c r="B27" s="20"/>
+      <c r="A27" s="21"/>
+      <c r="B27" s="19"/>
       <c r="C27" s="4"/>
       <c r="D27" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E27" s="79" t="s">
+      <c r="E27" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="F27" s="80"/>
+      <c r="F27" s="64"/>
       <c r="G27" s="8" t="s">
         <v>14</v>
       </c>
       <c r="H27" s="4"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="20"/>
-      <c r="O27" s="21"/>
-      <c r="P27" s="20"/>
-      <c r="Q27" s="20"/>
-      <c r="R27" s="20"/>
-      <c r="S27" s="20"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="20"/>
+      <c r="P27" s="19"/>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="19"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" s="22"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
-      <c r="K28" s="24"/>
-      <c r="L28" s="24"/>
-      <c r="M28" s="24"/>
-      <c r="N28" s="24"/>
-      <c r="O28" s="21"/>
-      <c r="P28" s="20"/>
-      <c r="Q28" s="20"/>
-      <c r="R28" s="20"/>
-      <c r="S28" s="20"/>
+      <c r="A28" s="21"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="23"/>
+      <c r="O28" s="20"/>
+      <c r="P28" s="19"/>
+      <c r="Q28" s="19"/>
+      <c r="R28" s="19"/>
+      <c r="S28" s="19"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
@@ -1850,12 +1807,23 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="C25:C26"/>
+  <mergeCells count="34">
+    <mergeCell ref="AD13:AD14"/>
+    <mergeCell ref="AA16:AB16"/>
+    <mergeCell ref="W16:X16"/>
+    <mergeCell ref="U14:U15"/>
+    <mergeCell ref="U12:U13"/>
+    <mergeCell ref="AE11:AK11"/>
+    <mergeCell ref="AE12:AK12"/>
+    <mergeCell ref="AE13:AK13"/>
+    <mergeCell ref="V10:Y10"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="U8:AC8"/>
+    <mergeCell ref="V11:W11"/>
+    <mergeCell ref="X11:Y11"/>
+    <mergeCell ref="Z11:AA11"/>
+    <mergeCell ref="AB11:AC11"/>
+    <mergeCell ref="Z10:AC10"/>
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="J13:N13"/>
     <mergeCell ref="J14:N14"/>
@@ -1867,53 +1835,16 @@
     <mergeCell ref="J24:N24"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="H15:H16"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="C25:C26"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="C16:C17"/>
-    <mergeCell ref="V10:Y10"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="U8:AC8"/>
-    <mergeCell ref="V11:W11"/>
-    <mergeCell ref="X11:Y11"/>
-    <mergeCell ref="Z11:AA11"/>
-    <mergeCell ref="AB11:AC11"/>
-    <mergeCell ref="Z10:AC10"/>
-    <mergeCell ref="AE11:AJ11"/>
-    <mergeCell ref="AD13:AD14"/>
-    <mergeCell ref="AA16:AB16"/>
-    <mergeCell ref="W16:X16"/>
-    <mergeCell ref="U14:U15"/>
-    <mergeCell ref="U12:U13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
-  <oleObjects>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <oleObject progId="Equation.3" shapeId="1025" r:id="rId4">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId5">
-            <anchor moveWithCells="1" sizeWithCells="1">
-              <from>
-                <xdr:col>31</xdr:col>
-                <xdr:colOff>400050</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>34</xdr:col>
-                <xdr:colOff>390525</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </to>
-            </anchor>
-          </objectPr>
-        </oleObject>
-      </mc:Choice>
-      <mc:Fallback>
-        <oleObject progId="Equation.3" shapeId="1025" r:id="rId4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-  </oleObjects>
 </worksheet>
 </file>
</xml_diff>